<commit_message>
evaluation graph is completed
</commit_message>
<xml_diff>
--- a/database/MainDataset.xlsx
+++ b/database/MainDataset.xlsx
@@ -21,22 +21,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Affected Age (0 - 3 = 0) (4 - 6 = 1) (6 - 9 = 2)</t>
+    <t>AffectedAge</t>
   </si>
   <si>
-    <t>Marriage Age of Mother</t>
+    <t>MarriageAgeMother</t>
   </si>
   <si>
-    <t>Age of Delivery</t>
+    <t>AgeOfDelivery</t>
   </si>
   <si>
-    <t>Disease during Pregnancy (Yes=1, No=0)</t>
+    <t>DiseaseDuringPregnancy</t>
   </si>
   <si>
-    <t>Disease (0, 1)</t>
+    <t>Disease</t>
   </si>
   <si>
-    <t>Chicken Pox (0), Malaria (1), Diarrhea (2), No Disease (3)</t>
+    <t>DiseaseName</t>
   </si>
 </sst>
 </file>
@@ -404,18 +404,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1201"/>
+  <dimension ref="A1:F1220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1183" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1165" workbookViewId="0">
+      <selection activeCell="A1181" sqref="A1181:F1220"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24021,22 +24023,22 @@
     </row>
     <row r="1181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1181">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1181">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1181">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1181">
         <v>1</v>
       </c>
       <c r="F1181">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1182" spans="1:6" x14ac:dyDescent="0.25">
@@ -24044,19 +24046,19 @@
         <v>2</v>
       </c>
       <c r="B1182">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C1182">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D1182">
         <v>0</v>
       </c>
       <c r="E1182">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1182">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1183" spans="1:6" x14ac:dyDescent="0.25">
@@ -24064,10 +24066,10 @@
         <v>0</v>
       </c>
       <c r="B1183">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C1183">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1183">
         <v>1</v>
@@ -24081,53 +24083,53 @@
     </row>
     <row r="1184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1184">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C1184">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D1184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1184">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1185">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C1185">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D1185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1185">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1186">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1186">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1186">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1186">
         <v>0</v>
@@ -24141,13 +24143,13 @@
     </row>
     <row r="1187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1187">
         <v>16</v>
       </c>
       <c r="C1187">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D1187">
         <v>1</v>
@@ -24156,55 +24158,55 @@
         <v>1</v>
       </c>
       <c r="F1187">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1188">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1188">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D1188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1188">
         <v>1</v>
       </c>
       <c r="F1188">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1189">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1189">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1189">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1189">
         <v>0</v>
       </c>
       <c r="E1189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1189">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1190">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1190">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C1190">
         <v>23</v>
@@ -24221,53 +24223,53 @@
     </row>
     <row r="1191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1191">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1191">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C1191">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D1191">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1191">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1191">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1192">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1192">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1192">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D1192">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1192">
         <v>1</v>
       </c>
       <c r="F1192">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1193">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1193">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C1193">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1193">
         <v>1</v>
@@ -24281,82 +24283,82 @@
     </row>
     <row r="1194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1194">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1194">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C1194">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1194">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1194">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1194">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1195">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1195">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C1195">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D1195">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1195">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1195">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1196">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1196">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C1196">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D1196">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1196">
         <v>1</v>
       </c>
       <c r="F1196">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1197">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1197">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1197">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1197">
         <v>1</v>
       </c>
       <c r="F1197">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1198" spans="1:6" x14ac:dyDescent="0.25">
@@ -24364,10 +24366,10 @@
         <v>1</v>
       </c>
       <c r="B1198">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1198">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1198">
         <v>1</v>
@@ -24384,10 +24386,10 @@
         <v>1</v>
       </c>
       <c r="B1199">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C1199">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1199">
         <v>1</v>
@@ -24404,39 +24406,419 @@
         <v>0</v>
       </c>
       <c r="B1200">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C1200">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D1200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1200">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1201">
+        <v>20</v>
+      </c>
+      <c r="C1201">
+        <v>24</v>
+      </c>
+      <c r="D1201">
+        <v>0</v>
+      </c>
+      <c r="E1201">
+        <v>1</v>
+      </c>
+      <c r="F1201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1202">
+        <v>2</v>
+      </c>
+      <c r="B1202">
+        <v>19</v>
+      </c>
+      <c r="C1202">
+        <v>18</v>
+      </c>
+      <c r="D1202">
+        <v>0</v>
+      </c>
+      <c r="E1202">
+        <v>1</v>
+      </c>
+      <c r="F1202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1203">
+        <v>1</v>
+      </c>
+      <c r="B1203">
+        <v>17</v>
+      </c>
+      <c r="C1203">
+        <v>23</v>
+      </c>
+      <c r="D1203">
+        <v>0</v>
+      </c>
+      <c r="E1203">
+        <v>1</v>
+      </c>
+      <c r="F1203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1204">
+        <v>1</v>
+      </c>
+      <c r="B1204">
+        <v>21</v>
+      </c>
+      <c r="C1204">
+        <v>19</v>
+      </c>
+      <c r="D1204">
+        <v>1</v>
+      </c>
+      <c r="E1204">
+        <v>1</v>
+      </c>
+      <c r="F1204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1205">
+        <v>0</v>
+      </c>
+      <c r="B1205">
+        <v>25</v>
+      </c>
+      <c r="C1205">
+        <v>24</v>
+      </c>
+      <c r="D1205">
+        <v>1</v>
+      </c>
+      <c r="E1205">
+        <v>0</v>
+      </c>
+      <c r="F1205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1206">
+        <v>0</v>
+      </c>
+      <c r="B1206">
+        <v>14</v>
+      </c>
+      <c r="C1206">
+        <v>16</v>
+      </c>
+      <c r="D1206">
+        <v>1</v>
+      </c>
+      <c r="E1206">
+        <v>1</v>
+      </c>
+      <c r="F1206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1207">
+        <v>1</v>
+      </c>
+      <c r="B1207">
         <v>26</v>
       </c>
-      <c r="C1201">
-        <v>26</v>
-      </c>
-      <c r="D1201">
-        <v>0</v>
-      </c>
-      <c r="E1201">
-        <v>0</v>
-      </c>
-      <c r="F1201">
-        <v>3</v>
+      <c r="C1207">
+        <v>27</v>
+      </c>
+      <c r="D1207">
+        <v>0</v>
+      </c>
+      <c r="E1207">
+        <v>0</v>
+      </c>
+      <c r="F1207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1208">
+        <v>1</v>
+      </c>
+      <c r="B1208">
+        <v>17</v>
+      </c>
+      <c r="C1208">
+        <v>24</v>
+      </c>
+      <c r="D1208">
+        <v>0</v>
+      </c>
+      <c r="E1208">
+        <v>1</v>
+      </c>
+      <c r="F1208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1209">
+        <v>1</v>
+      </c>
+      <c r="B1209">
+        <v>17</v>
+      </c>
+      <c r="C1209">
+        <v>24</v>
+      </c>
+      <c r="D1209">
+        <v>0</v>
+      </c>
+      <c r="E1209">
+        <v>1</v>
+      </c>
+      <c r="F1209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1210">
+        <v>0</v>
+      </c>
+      <c r="B1210">
+        <v>14</v>
+      </c>
+      <c r="C1210">
+        <v>15</v>
+      </c>
+      <c r="D1210">
+        <v>1</v>
+      </c>
+      <c r="E1210">
+        <v>1</v>
+      </c>
+      <c r="F1210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1211">
+        <v>2</v>
+      </c>
+      <c r="B1211">
+        <v>28</v>
+      </c>
+      <c r="C1211">
+        <v>28</v>
+      </c>
+      <c r="D1211">
+        <v>0</v>
+      </c>
+      <c r="E1211">
+        <v>0</v>
+      </c>
+      <c r="F1211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1212">
+        <v>1</v>
+      </c>
+      <c r="B1212">
+        <v>20</v>
+      </c>
+      <c r="C1212">
+        <v>24</v>
+      </c>
+      <c r="D1212">
+        <v>0</v>
+      </c>
+      <c r="E1212">
+        <v>1</v>
+      </c>
+      <c r="F1212">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1213">
+        <v>0</v>
+      </c>
+      <c r="B1213">
+        <v>14</v>
+      </c>
+      <c r="C1213">
+        <v>16</v>
+      </c>
+      <c r="D1213">
+        <v>1</v>
+      </c>
+      <c r="E1213">
+        <v>1</v>
+      </c>
+      <c r="F1213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1214">
+        <v>0</v>
+      </c>
+      <c r="B1214">
+        <v>14</v>
+      </c>
+      <c r="C1214">
+        <v>15</v>
+      </c>
+      <c r="D1214">
+        <v>1</v>
+      </c>
+      <c r="E1214">
+        <v>1</v>
+      </c>
+      <c r="F1214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1215">
+        <v>0</v>
+      </c>
+      <c r="B1215">
+        <v>14</v>
+      </c>
+      <c r="C1215">
+        <v>16</v>
+      </c>
+      <c r="D1215">
+        <v>1</v>
+      </c>
+      <c r="E1215">
+        <v>1</v>
+      </c>
+      <c r="F1215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1216">
+        <v>0</v>
+      </c>
+      <c r="B1216">
+        <v>15</v>
+      </c>
+      <c r="C1216">
+        <v>18</v>
+      </c>
+      <c r="D1216">
+        <v>1</v>
+      </c>
+      <c r="E1216">
+        <v>1</v>
+      </c>
+      <c r="F1216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1217">
+        <v>1</v>
+      </c>
+      <c r="B1217">
+        <v>30</v>
+      </c>
+      <c r="C1217">
+        <v>22</v>
+      </c>
+      <c r="D1217">
+        <v>0</v>
+      </c>
+      <c r="E1217">
+        <v>0</v>
+      </c>
+      <c r="F1217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1218">
+        <v>1</v>
+      </c>
+      <c r="B1218">
+        <v>16</v>
+      </c>
+      <c r="C1218">
+        <v>19</v>
+      </c>
+      <c r="D1218">
+        <v>1</v>
+      </c>
+      <c r="E1218">
+        <v>1</v>
+      </c>
+      <c r="F1218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1219">
+        <v>1</v>
+      </c>
+      <c r="B1219">
+        <v>17</v>
+      </c>
+      <c r="C1219">
+        <v>24</v>
+      </c>
+      <c r="D1219">
+        <v>0</v>
+      </c>
+      <c r="E1219">
+        <v>1</v>
+      </c>
+      <c r="F1219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1220">
+        <v>0</v>
+      </c>
+      <c r="B1220">
+        <v>14</v>
+      </c>
+      <c r="C1220">
+        <v>16</v>
+      </c>
+      <c r="D1220">
+        <v>1</v>
+      </c>
+      <c r="E1220">
+        <v>1</v>
+      </c>
+      <c r="F1220">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All graph is calculated
</commit_message>
<xml_diff>
--- a/database/MainDataset.xlsx
+++ b/database/MainDataset.xlsx
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1165" workbookViewId="0">
-      <selection activeCell="A1181" sqref="A1181:F1220"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>